<commit_message>
Updated M1 results for DiffRed on Bank
</commit_message>
<xml_diff>
--- a/Experiments/dimensionality_reduction_metrics/results/M1_results/Bank.xlsx
+++ b/Experiments/dimensionality_reduction_metrics/results/M1_results/Bank.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,1005 @@
         <v>9.474574336643116e-06</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:46</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.0003567146545742084</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:46</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.000192279810876439</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:46</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.002623358033710388</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:46</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="n">
+        <v>6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" t="n">
+        <v>3.601296887278949e-05</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:46</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.001685338338723197</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" t="n">
+        <v>6</v>
+      </c>
+      <c r="E12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" t="n">
+        <v>4.572818349535268e-07</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
+        <v>4</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>5.819229140002768e-06</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" t="n">
+        <v>7</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.939089298030883e-05</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>100</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>6</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.003607092065443296</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>100</v>
+      </c>
+      <c r="D16" t="n">
+        <v>7</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>7</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.01178359939171436</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:47</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>100</v>
+      </c>
+      <c r="D17" t="n">
+        <v>7</v>
+      </c>
+      <c r="E17" t="n">
+        <v>4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>3</v>
+      </c>
+      <c r="G17" t="n">
+        <v>3.312755135098655e-06</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>100</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.006966345516345562</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>100</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F19" t="n">
+        <v>5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.004556227912715594</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>100</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>5</v>
+      </c>
+      <c r="F20" t="n">
+        <v>3</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.06064296462916e-06</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>100</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6</v>
+      </c>
+      <c r="E21" t="n">
+        <v>4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>2.920821435736798e-05</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>100</v>
+      </c>
+      <c r="D22" t="n">
+        <v>8</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="n">
+        <v>6</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0001174635325487117</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:48</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3</v>
+      </c>
+      <c r="F23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.0001483777378356033</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D24" t="n">
+        <v>7</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>4</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.000287218250922705</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2.508717329552379e-05</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>100</v>
+      </c>
+      <c r="D26" t="n">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.0006347474575996159</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>100</v>
+      </c>
+      <c r="D27" t="n">
+        <v>8</v>
+      </c>
+      <c r="E27" t="n">
+        <v>7</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1</v>
+      </c>
+      <c r="G27" t="n">
+        <v>3.485003710057555e-07</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>100</v>
+      </c>
+      <c r="D28" t="n">
+        <v>7</v>
+      </c>
+      <c r="E28" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" t="n">
+        <v>9.221067224562951e-06</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:49</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>100</v>
+      </c>
+      <c r="D29" t="n">
+        <v>5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>5</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.002059371255043074</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2.823645841187883e-05</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>100</v>
+      </c>
+      <c r="D31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.012332367122948e-05</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>100</v>
+      </c>
+      <c r="D32" t="n">
+        <v>8</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>2</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3.574125952643392e-06</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>100</v>
+      </c>
+      <c r="D33" t="n">
+        <v>8</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F33" t="n">
+        <v>5</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2.538276654395766e-05</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>100</v>
+      </c>
+      <c r="D34" t="n">
+        <v>7</v>
+      </c>
+      <c r="E34" t="n">
+        <v>5</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2.592921699129391e-06</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:50</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>100</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>8</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.001773838885955836</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>100</v>
+      </c>
+      <c r="D36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.01220146782455322</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>100</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.01250813688425967</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.003476397239279616</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>100</v>
+      </c>
+      <c r="D39" t="n">
+        <v>10</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="n">
+        <v>8</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.0001378989805362885</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>100</v>
+      </c>
+      <c r="D40" t="n">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4</v>
+      </c>
+      <c r="F40" t="n">
+        <v>6</v>
+      </c>
+      <c r="G40" t="n">
+        <v>6.895691803787685e-06</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>100</v>
+      </c>
+      <c r="D41" t="n">
+        <v>10</v>
+      </c>
+      <c r="E41" t="n">
+        <v>5</v>
+      </c>
+      <c r="F41" t="n">
+        <v>5</v>
+      </c>
+      <c r="G41" t="n">
+        <v>9.474574336643116e-06</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>100</v>
+      </c>
+      <c r="D42" t="n">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="n">
+        <v>3</v>
+      </c>
+      <c r="G42" t="n">
+        <v>1.146297581189337e-06</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2023-10-08 21:58:51</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>100</v>
+      </c>
+      <c r="D43" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" t="n">
+        <v>8</v>
+      </c>
+      <c r="F43" t="n">
+        <v>2</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.782396432670197e-07</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>